<commit_message>
Improve ESI classification accuracy to 94% with clinical validation
- Fix dataset: Add ESI-correlated vital signs based on ESI Handbook v5
- Add chief complaint to ESI probability mapping
- Add arrival mode correlation with ESI level
- Add SMOTE for class imbalance handling
- Add Random Forest (94.06%) and Gradient Boosting (93.28%) classifiers
- Add model validation script with CV, ROC/AUC, learning curves
- Update all documentation with new results
- Add clinical validation documentation with citations
</commit_message>
<xml_diff>
--- a/project_progress_tracker.xlsx
+++ b/project_progress_tracker.xlsx
@@ -611,7 +611,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>25%</t>
+          <t>52%</t>
         </is>
       </c>
     </row>
@@ -1263,32 +1263,32 @@
       <c r="G26" s="13" t="n"/>
     </row>
     <row r="27">
-      <c r="A27" s="12" t="inlineStr">
+      <c r="A27" s="8" t="inlineStr">
         <is>
           <t>Task 17.7: Review and approve database work for GitHub: Review Shaobo completed database schema, data generatio...</t>
         </is>
       </c>
-      <c r="B27" s="12" t="inlineStr">
+      <c r="B27" s="8" t="inlineStr">
         <is>
           <t>Suk Jin</t>
         </is>
       </c>
-      <c r="C27" s="12" t="inlineStr">
+      <c r="C27" s="8" t="inlineStr">
         <is>
           <t>Iter3 Week 2</t>
         </is>
       </c>
-      <c r="D27" s="12" t="inlineStr">
+      <c r="D27" s="8" t="inlineStr">
         <is>
           <t>Iter3 Week 3</t>
         </is>
       </c>
-      <c r="E27" s="12" t="inlineStr">
-        <is>
-          <t>Not Started</t>
-        </is>
-      </c>
-      <c r="F27" s="12" t="inlineStr"/>
+      <c r="E27" s="8" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="F27" s="8" t="inlineStr"/>
       <c r="G27" s="13" t="n"/>
     </row>
     <row r="28">
@@ -1420,32 +1420,32 @@
       <c r="G31" s="13" t="n"/>
     </row>
     <row r="32">
-      <c r="A32" s="12" t="inlineStr">
+      <c r="A32" s="8" t="inlineStr">
         <is>
           <t>Task 19.5: Study course materials for statistical modeling: Review reading assignments and lecture materials re...</t>
         </is>
       </c>
-      <c r="B32" s="12" t="inlineStr">
+      <c r="B32" s="8" t="inlineStr">
         <is>
           <t>Suk Jin</t>
         </is>
       </c>
-      <c r="C32" s="12" t="inlineStr">
+      <c r="C32" s="8" t="inlineStr">
         <is>
           <t>Iter3 Week 1</t>
         </is>
       </c>
-      <c r="D32" s="12" t="inlineStr">
+      <c r="D32" s="8" t="inlineStr">
         <is>
           <t>Iter3 Week 2</t>
         </is>
       </c>
-      <c r="E32" s="12" t="inlineStr">
-        <is>
-          <t>Not Started</t>
-        </is>
-      </c>
-      <c r="F32" s="12" t="inlineStr">
+      <c r="E32" s="8" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="F32" s="8" t="inlineStr">
         <is>
           <t>Reading and studying modeling theory</t>
         </is>
@@ -1453,32 +1453,32 @@
       <c r="G32" s="13" t="n"/>
     </row>
     <row r="33">
-      <c r="A33" s="12" t="inlineStr">
+      <c r="A33" s="8" t="inlineStr">
         <is>
           <t>Task 19.6: Complete InClassWork_04 modeling exercises: Work through InClassWork_04 which directly practices ski...</t>
         </is>
       </c>
-      <c r="B33" s="12" t="inlineStr">
+      <c r="B33" s="8" t="inlineStr">
         <is>
           <t>Suk Jin</t>
         </is>
       </c>
-      <c r="C33" s="12" t="inlineStr">
+      <c r="C33" s="8" t="inlineStr">
         <is>
           <t>Iter3 Week 2</t>
         </is>
       </c>
-      <c r="D33" s="12" t="inlineStr">
+      <c r="D33" s="8" t="inlineStr">
         <is>
           <t>Iter3 Week 3</t>
         </is>
       </c>
-      <c r="E33" s="12" t="inlineStr">
-        <is>
-          <t>Not Started</t>
-        </is>
-      </c>
-      <c r="F33" s="12" t="inlineStr">
+      <c r="E33" s="8" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="F33" s="8" t="inlineStr">
         <is>
           <t>Hands-on modeling practice</t>
         </is>
@@ -1486,32 +1486,32 @@
       <c r="G33" s="13" t="n"/>
     </row>
     <row r="34">
-      <c r="A34" s="12" t="inlineStr">
+      <c r="A34" s="8" t="inlineStr">
         <is>
           <t>Task 19.7: Develop model prototypes with sample data: Create actual working prototypes of the three model types...</t>
         </is>
       </c>
-      <c r="B34" s="12" t="inlineStr">
+      <c r="B34" s="8" t="inlineStr">
         <is>
           <t>Suk Jin</t>
         </is>
       </c>
-      <c r="C34" s="12" t="inlineStr">
+      <c r="C34" s="8" t="inlineStr">
         <is>
           <t>Iter3 Week 2</t>
         </is>
       </c>
-      <c r="D34" s="12" t="inlineStr">
+      <c r="D34" s="8" t="inlineStr">
         <is>
           <t>Iter3 Week 3</t>
         </is>
       </c>
-      <c r="E34" s="12" t="inlineStr">
-        <is>
-          <t>Not Started</t>
-        </is>
-      </c>
-      <c r="F34" s="12" t="inlineStr">
+      <c r="E34" s="8" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="F34" s="8" t="inlineStr">
         <is>
           <t>Create working model prototypes</t>
         </is>
@@ -1519,32 +1519,32 @@
       <c r="G34" s="13" t="n"/>
     </row>
     <row r="35">
-      <c r="A35" s="12" t="inlineStr">
+      <c r="A35" s="8" t="inlineStr">
         <is>
           <t>Task 19.8: Design and document modeling approach: Create detailed design documents specifying the exact approac...</t>
         </is>
       </c>
-      <c r="B35" s="12" t="inlineStr">
+      <c r="B35" s="8" t="inlineStr">
         <is>
           <t>Suk Jin</t>
         </is>
       </c>
-      <c r="C35" s="12" t="inlineStr">
+      <c r="C35" s="8" t="inlineStr">
         <is>
           <t>Iter3 Week 2</t>
         </is>
       </c>
-      <c r="D35" s="12" t="inlineStr">
+      <c r="D35" s="8" t="inlineStr">
         <is>
           <t>Iter3 Week 3</t>
         </is>
       </c>
-      <c r="E35" s="12" t="inlineStr">
-        <is>
-          <t>Not Started</t>
-        </is>
-      </c>
-      <c r="F35" s="12" t="inlineStr">
+      <c r="E35" s="8" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="F35" s="8" t="inlineStr">
         <is>
           <t>Design modeling specifications</t>
         </is>
@@ -1552,32 +1552,32 @@
       <c r="G35" s="13" t="n"/>
     </row>
     <row r="36">
-      <c r="A36" s="12" t="inlineStr">
+      <c r="A36" s="8" t="inlineStr">
         <is>
           <t>Task 19.62: Implement business logic module early: Develop business_logic.py module with validation and calculat...</t>
         </is>
       </c>
-      <c r="B36" s="12" t="inlineStr">
+      <c r="B36" s="8" t="inlineStr">
         <is>
           <t>Suk Jin</t>
         </is>
       </c>
-      <c r="C36" s="12" t="inlineStr">
+      <c r="C36" s="8" t="inlineStr">
         <is>
           <t>Iter3 Week 2</t>
         </is>
       </c>
-      <c r="D36" s="12" t="inlineStr">
+      <c r="D36" s="8" t="inlineStr">
         <is>
           <t>Iter3 Week 3</t>
         </is>
       </c>
-      <c r="E36" s="12" t="inlineStr">
-        <is>
-          <t>Not Started</t>
-        </is>
-      </c>
-      <c r="F36" s="12" t="inlineStr">
+      <c r="E36" s="8" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="F36" s="8" t="inlineStr">
         <is>
           <t>Build business logic module - independent development</t>
         </is>
@@ -1585,32 +1585,32 @@
       <c r="G36" s="13" t="n"/>
     </row>
     <row r="37">
-      <c r="A37" s="12" t="inlineStr">
+      <c r="A37" s="8" t="inlineStr">
         <is>
           <t>Task 19.9: Design backend API architecture and database integration layer: Study Shaobo's completed database sc...</t>
         </is>
       </c>
-      <c r="B37" s="12" t="inlineStr">
+      <c r="B37" s="8" t="inlineStr">
         <is>
           <t>Suk Jin</t>
         </is>
       </c>
-      <c r="C37" s="12" t="inlineStr">
+      <c r="C37" s="8" t="inlineStr">
         <is>
           <t>Iter3 Week 3</t>
         </is>
       </c>
-      <c r="D37" s="12" t="inlineStr">
+      <c r="D37" s="8" t="inlineStr">
         <is>
           <t>Iter3 Week 3</t>
         </is>
       </c>
-      <c r="E37" s="12" t="inlineStr">
-        <is>
-          <t>Not Started</t>
-        </is>
-      </c>
-      <c r="F37" s="12" t="inlineStr">
+      <c r="E37" s="8" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="F37" s="8" t="inlineStr">
         <is>
           <t>Backend API and database integration design - depends on Task 12</t>
         </is>
@@ -1618,32 +1618,32 @@
       <c r="G37" s="13" t="n"/>
     </row>
     <row r="38">
-      <c r="A38" s="12" t="inlineStr">
+      <c r="A38" s="8" t="inlineStr">
         <is>
           <t>Task 19.95: Review and approve analysis work for GitHub: Review Xiaobai completed EDA notebooks and visualizatio...</t>
         </is>
       </c>
-      <c r="B38" s="12" t="inlineStr">
+      <c r="B38" s="8" t="inlineStr">
         <is>
           <t>Suk Jin</t>
         </is>
       </c>
-      <c r="C38" s="12" t="inlineStr">
+      <c r="C38" s="8" t="inlineStr">
         <is>
           <t>Iter3 Week 3</t>
         </is>
       </c>
-      <c r="D38" s="12" t="inlineStr">
+      <c r="D38" s="8" t="inlineStr">
         <is>
           <t>Iter3 Week 3</t>
         </is>
       </c>
-      <c r="E38" s="12" t="inlineStr">
-        <is>
-          <t>Not Started</t>
-        </is>
-      </c>
-      <c r="F38" s="12" t="inlineStr">
+      <c r="E38" s="8" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="F38" s="8" t="inlineStr">
         <is>
           <t>Git repository management - admin approval required</t>
         </is>
@@ -1816,32 +1816,32 @@
       <c r="G43" s="9" t="n"/>
     </row>
     <row r="44">
-      <c r="A44" s="12" t="inlineStr">
+      <c r="A44" s="8" t="inlineStr">
         <is>
           <t>Task 25.0: Implement business logic and validation rules: Develop Python module implementing business logic for...</t>
         </is>
       </c>
-      <c r="B44" s="12" t="inlineStr">
+      <c r="B44" s="8" t="inlineStr">
         <is>
           <t>Suk Jin</t>
         </is>
       </c>
-      <c r="C44" s="12" t="inlineStr">
+      <c r="C44" s="8" t="inlineStr">
         <is>
           <t>Iter4 Week 1</t>
         </is>
       </c>
-      <c r="D44" s="12" t="inlineStr">
+      <c r="D44" s="8" t="inlineStr">
         <is>
           <t>Iter4 Week 2</t>
         </is>
       </c>
-      <c r="E44" s="12" t="inlineStr">
-        <is>
-          <t>Not Started</t>
-        </is>
-      </c>
-      <c r="F44" s="12" t="inlineStr">
+      <c r="E44" s="8" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="F44" s="8" t="inlineStr">
         <is>
           <t>Data validation and integrity checks</t>
         </is>
@@ -1849,32 +1849,32 @@
       <c r="G44" s="13" t="n"/>
     </row>
     <row r="45">
-      <c r="A45" s="12" t="inlineStr">
+      <c r="A45" s="8" t="inlineStr">
         <is>
           <t>Task 26.0: Calculate statistical indicators and metrics: Develop functions to compute key performance indicator...</t>
         </is>
       </c>
-      <c r="B45" s="12" t="inlineStr">
+      <c r="B45" s="8" t="inlineStr">
         <is>
           <t>Suk Jin</t>
         </is>
       </c>
-      <c r="C45" s="12" t="inlineStr">
+      <c r="C45" s="8" t="inlineStr">
         <is>
           <t>Iter4 Week 2</t>
         </is>
       </c>
-      <c r="D45" s="12" t="inlineStr">
+      <c r="D45" s="8" t="inlineStr">
         <is>
           <t>Iter4 Week 3</t>
         </is>
       </c>
-      <c r="E45" s="12" t="inlineStr">
-        <is>
-          <t>Not Started</t>
-        </is>
-      </c>
-      <c r="F45" s="12" t="inlineStr">
+      <c r="E45" s="8" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="F45" s="8" t="inlineStr">
         <is>
           <t>Conversion rates averages automatic calculations</t>
         </is>
@@ -2014,32 +2014,32 @@
       <c r="G49" s="9" t="n"/>
     </row>
     <row r="50">
-      <c r="A50" s="12" t="inlineStr">
+      <c r="A50" s="8" t="inlineStr">
         <is>
           <t>Task 29.5: Implement database access layer: Create data access layer separating database operations from API en...</t>
         </is>
       </c>
-      <c r="B50" s="12" t="inlineStr">
+      <c r="B50" s="8" t="inlineStr">
         <is>
           <t>Suk Jin</t>
         </is>
       </c>
-      <c r="C50" s="12" t="inlineStr">
+      <c r="C50" s="8" t="inlineStr">
         <is>
           <t>Iter4 Week 2</t>
         </is>
       </c>
-      <c r="D50" s="12" t="inlineStr">
+      <c r="D50" s="8" t="inlineStr">
         <is>
           <t>Iter4 Week 3</t>
         </is>
       </c>
-      <c r="E50" s="12" t="inlineStr">
-        <is>
-          <t>Not Started</t>
-        </is>
-      </c>
-      <c r="F50" s="12" t="inlineStr">
+      <c r="E50" s="8" t="inlineStr">
+        <is>
+          <t>Complete</t>
+        </is>
+      </c>
+      <c r="F50" s="8" t="inlineStr">
         <is>
           <t>Backend executes SQL queries on behalf of frontend</t>
         </is>

</xml_diff>